<commit_message>
bổ sung hàm getExcelData để đọc tất cả các dòng trong 1 sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest_CRM/datatest.xlsx
+++ b/src/test/resources/datatest_CRM/datatest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DemoSeleniumJavaOrangeHRM\src\test\resources\datatest_OrangeHRM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DemoDuAnCuoiKhoaCRM\src\test\resources\datatest_CRM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>EMAIL</t>
   </si>
@@ -36,9 +36,6 @@
     <t>admin@example.com</t>
   </si>
   <si>
-    <t>user@gmail.com</t>
-  </si>
-  <si>
     <t>CUSTOMER_NAME</t>
   </si>
   <si>
@@ -70,13 +67,16 @@
   </si>
   <si>
     <t>giangtest.com</t>
+  </si>
+  <si>
+    <t>admin1@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +88,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,10 +120,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -399,9 +411,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -420,7 +432,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2">
@@ -428,19 +440,27 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1253</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -448,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,44 +482,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update code getDataHashTable ghi log
</commit_message>
<xml_diff>
--- a/src/test/resources/datatest_CRM/datatest.xlsx
+++ b/src/test/resources/datatest_CRM/datatest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>EMAIL</t>
   </si>
@@ -69,7 +69,16 @@
     <t>giangtest.com</t>
   </si>
   <si>
-    <t>admin1@example.com</t>
+    <t>user@example.com</t>
+  </si>
+  <si>
+    <t>customer1@example.com</t>
+  </si>
+  <si>
+    <t>hatest@example.com</t>
+  </si>
+  <si>
+    <t>hatest2@example.com</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,8 +449,8 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
+      <c r="A3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1253</v>
@@ -449,18 +458,53 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3434</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>